<commit_message>
new speedup diagram in presentation
</commit_message>
<xml_diff>
--- a/presentation/grafiken.xlsx
+++ b/presentation/grafiken.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="8160"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Zeitanteil</t>
   </si>
@@ -61,13 +61,16 @@
   <si>
     <t>Amdahls law</t>
   </si>
+  <si>
+    <t>vi ho</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -101,7 +104,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -505,7 +508,496 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Speedup</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="34925">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$I$3,Tabelle1!$I$4,Tabelle1!$I$5,Tabelle1!$I$6,Tabelle1!$I$8,Tabelle1!$I$10,Tabelle1!$I$11,Tabelle1!$I$14,Tabelle1!$I$18)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$N$3,Tabelle1!$N$4,Tabelle1!$N$5,Tabelle1!$N$6,Tabelle1!$N$8,Tabelle1!$N$10,Tabelle1!$N$11,Tabelle1!$N$14,Tabelle1!$N$18)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4858687041006275</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7547597591564736</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8894976745623384</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1585158773586572</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.269572834850262</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0898371010411041</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1480284421460891</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5063824554211926</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Optimaler Speedup nach Amdahl</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="3175" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$O$3:$O$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.480101137371808</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7620958832785452</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.94763108752175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0789709190515437</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1768351622008599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2525754476968598</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3129321566897372</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3621600274725276</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4030772241941132</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.4376244499195763</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4671817904558742</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4927575137580269</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.515105385556736</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.5348002031934986</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.552287935524082</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="435021000"/>
+        <c:axId val="435025704"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="435021000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="16"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435025704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="435025704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2.6"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435021000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1047,6 +1539,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1074,6 +2082,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1347,8 +2385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N18"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,7 +2496,22 @@
       <c r="I5">
         <v>3</v>
       </c>
-      <c r="N5" s="1"/>
+      <c r="J5">
+        <v>7.0115999999999998E-2</v>
+      </c>
+      <c r="K5">
+        <v>0.14602000000000001</v>
+      </c>
+      <c r="L5">
+        <v>0.13190099999999999</v>
+      </c>
+      <c r="M5">
+        <v>0.34844199999999997</v>
+      </c>
+      <c r="N5" s="1">
+        <f>M3/M5</f>
+        <v>1.7547597591564736</v>
+      </c>
       <c r="O5" s="1">
         <f>1/(J21+1/I5*(1-J21))</f>
         <v>1.7620958832785452</v>
@@ -1571,11 +2624,22 @@
       <c r="I11">
         <v>9</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="1"/>
+      <c r="J11" s="2">
+        <v>7.8631999999999994E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.16467300000000001</v>
+      </c>
+      <c r="L11" s="2">
+        <v>4.9140000000000003E-2</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0.292574</v>
+      </c>
+      <c r="N11" s="1">
+        <f>M3/M11</f>
+        <v>2.0898371010411041</v>
+      </c>
       <c r="O11" s="1">
         <f>1/(J21+1/I11*(1-J21))</f>
         <v>2.3621600274725276</v>
@@ -1613,11 +2677,22 @@
       <c r="I14">
         <v>12</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="1"/>
+      <c r="J14" s="2">
+        <v>7.9884999999999998E-2</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.16631299999999999</v>
+      </c>
+      <c r="L14" s="2">
+        <v>3.7344000000000002E-2</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.28464800000000001</v>
+      </c>
+      <c r="N14" s="1">
+        <f>M3/M14</f>
+        <v>2.1480284421460891</v>
+      </c>
       <c r="O14" s="1">
         <f>1/(J21+1/I14*(1-J21))</f>
         <v>2.4671817904558742</v>
@@ -1631,7 +2706,9 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="1"/>
+      <c r="N15" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="O15" s="1">
         <f>1/(J21+1/I15*(1-J21))</f>
         <v>2.4927575137580269</v>

</xml_diff>